<commit_message>
no changes; test commit
</commit_message>
<xml_diff>
--- a/Census Geog Reference v2.xlsx
+++ b/Census Geog Reference v2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr date1904="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Shared drives\Squeeze Project\Census Geography Reference\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDDCC203-DCEB-4BF6-8C3C-6A5D8F313A8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E1E0109-6341-43B0-AB8A-519EE6BEEC48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1247" yWindow="13" windowWidth="12246" windowHeight="7187" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13866" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Codebook" sheetId="8" r:id="rId1"/>
@@ -1516,15 +1516,15 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1588,7 +1588,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1603,7 +1603,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1710,7 +1710,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D95E557A-C484-485C-A175-A3BC7A948D84}" name="Table1" displayName="Table1" ref="B3:M55" totalsRowShown="0" headerRowDxfId="13" dataDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D95E557A-C484-485C-A175-A3BC7A948D84}" name="Table1" displayName="Table1" ref="B3:M55" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
   <autoFilter ref="B3:M55" xr:uid="{D95E557A-C484-485C-A175-A3BC7A948D84}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -1726,17 +1726,17 @@
     <filterColumn colId="11" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="12">
-    <tableColumn id="2" xr3:uid="{D103D2B8-ED19-49B9-B713-6FFAB2660C2D}" name="Abbr" dataDxfId="12"/>
-    <tableColumn id="1" xr3:uid="{8B3A9D89-FDC6-472D-9CE8-E6E9B40FC3CB}" name="States" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{96508804-287A-4E40-B5E5-61087FA7D949}" name="Non-governmental" dataDxfId="10"/>
-    <tableColumn id="13" xr3:uid="{AA70841F-C60E-4CA2-BBD6-EF69CC146631}" name="Governmental" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{46492768-2F6A-4B08-9570-05A9CE9A4289}" name="Unincorporated" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{274FB2C5-7DBE-4F9E-B057-89FB5F52D829}" name="Incorporated" dataDxfId="7"/>
-    <tableColumn id="8" xr3:uid="{DCE6B69C-7AAB-41FF-98F4-F39313CA0F65}" name="CSD" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{ED33F0F2-F213-4D90-8587-F30BFEC3DCF2}" name="Places" dataDxfId="3"/>
-    <tableColumn id="11" xr3:uid="{B1F8AB8D-FD3E-496B-B25B-8427C1D956CD}" name="CSD Duplicate" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{D103D2B8-ED19-49B9-B713-6FFAB2660C2D}" name="Abbr" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{8B3A9D89-FDC6-472D-9CE8-E6E9B40FC3CB}" name="States" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{96508804-287A-4E40-B5E5-61087FA7D949}" name="Non-governmental" dataDxfId="9"/>
+    <tableColumn id="13" xr3:uid="{AA70841F-C60E-4CA2-BBD6-EF69CC146631}" name="Governmental" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{46492768-2F6A-4B08-9570-05A9CE9A4289}" name="Unincorporated" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{274FB2C5-7DBE-4F9E-B057-89FB5F52D829}" name="Incorporated" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{DCE6B69C-7AAB-41FF-98F4-F39313CA0F65}" name="CSD" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{ED33F0F2-F213-4D90-8587-F30BFEC3DCF2}" name="Places" dataDxfId="4"/>
+    <tableColumn id="11" xr3:uid="{B1F8AB8D-FD3E-496B-B25B-8427C1D956CD}" name="CSD Duplicate" dataDxfId="3"/>
     <tableColumn id="10" xr3:uid="{F96F18AE-8378-4EBC-BF53-6F3FA5EED055}" name="Overlap" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{987E6162-B550-40FB-9768-A1BA5BF57A3C}" name="Notes" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{987E6162-B550-40FB-9768-A1BA5BF57A3C}" name="Notes" dataDxfId="1"/>
     <tableColumn id="12" xr3:uid="{0FFBBBF3-6F76-43F5-BE48-6F2790C73D3E}" name="Sources" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight6 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -3551,7 +3551,7 @@
   <dimension ref="B2:N55"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -3567,29 +3567,29 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" x14ac:dyDescent="0.5">
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="14" t="s">
         <v>289</v>
       </c>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11" t="s">
+      <c r="E2" s="14"/>
+      <c r="F2" s="14" t="s">
         <v>290</v>
       </c>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11" t="s">
+      <c r="G2" s="14"/>
+      <c r="H2" s="14" t="s">
         <v>298</v>
       </c>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-    </row>
-    <row r="3" spans="2:14" s="13" customFormat="1" ht="43" x14ac:dyDescent="0.5">
-      <c r="B3" s="13" t="s">
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
+    </row>
+    <row r="3" spans="2:14" s="12" customFormat="1" ht="43" x14ac:dyDescent="0.5">
+      <c r="B3" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="12" t="s">
         <v>287</v>
       </c>
       <c r="D3" s="9" t="s">
@@ -3616,972 +3616,972 @@
       <c r="K3" s="9" t="s">
         <v>236</v>
       </c>
-      <c r="L3" s="13" t="s">
+      <c r="L3" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="M3" s="13" t="s">
+      <c r="M3" s="12" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="4" spans="2:14" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="13" t="s">
         <v>294</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="G4" s="13" t="s">
         <v>295</v>
       </c>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14" t="s">
+      <c r="H4" s="13"/>
+      <c r="I4" s="13" t="s">
         <v>300</v>
       </c>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
     </row>
     <row r="5" spans="2:14" ht="86" x14ac:dyDescent="0.5">
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="13" t="s">
         <v>296</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="13" t="s">
         <v>294</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="F5" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="13" t="s">
         <v>297</v>
       </c>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14" t="s">
+      <c r="H5" s="13"/>
+      <c r="I5" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14" t="s">
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13" t="s">
         <v>302</v>
       </c>
-      <c r="M5" s="14" t="s">
+      <c r="M5" s="13" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.5">
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.5">
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="14"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.5">
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="14"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.5">
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="14"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.5">
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="14"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.5">
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="14"/>
-      <c r="M11" s="14"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="13"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.5">
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="14"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="13"/>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.5">
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="13"/>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.5">
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="14"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="13"/>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.5">
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="14"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="13"/>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.5">
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="14"/>
-      <c r="M16" s="14"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="13"/>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.5">
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="14"/>
-      <c r="M17" s="14"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="13"/>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.5">
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="14"/>
-      <c r="L18" s="14"/>
-      <c r="M18" s="14"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="13"/>
+      <c r="M18" s="13"/>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.5">
-      <c r="B19" s="13" t="s">
+      <c r="B19" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C19" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="14"/>
-      <c r="L19" s="14"/>
-      <c r="M19" s="14"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="13"/>
+      <c r="M19" s="13"/>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.5">
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C20" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
-      <c r="K20" s="14"/>
-      <c r="L20" s="14"/>
-      <c r="M20" s="14"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="13"/>
+      <c r="M20" s="13"/>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.5">
-      <c r="B21" s="13" t="s">
+      <c r="B21" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C21" s="13" t="s">
+      <c r="C21" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
-      <c r="K21" s="14"/>
-      <c r="L21" s="14"/>
-      <c r="M21" s="14"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13"/>
+      <c r="M21" s="13"/>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.5">
-      <c r="B22" s="13" t="s">
+      <c r="B22" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C22" s="13" t="s">
+      <c r="C22" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="14"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="14"/>
-      <c r="K22" s="14"/>
-      <c r="L22" s="14"/>
-      <c r="M22" s="14"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="13"/>
+      <c r="K22" s="13"/>
+      <c r="L22" s="13"/>
+      <c r="M22" s="13"/>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.5">
-      <c r="B23" s="13" t="s">
+      <c r="B23" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="13" t="s">
+      <c r="C23" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="14"/>
-      <c r="K23" s="14"/>
-      <c r="L23" s="14"/>
-      <c r="M23" s="14"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="13"/>
+      <c r="K23" s="13"/>
+      <c r="L23" s="13"/>
+      <c r="M23" s="13"/>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.5">
-      <c r="B24" s="13" t="s">
+      <c r="B24" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="13" t="s">
+      <c r="C24" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="14"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="14"/>
-      <c r="K24" s="14"/>
-      <c r="L24" s="14"/>
-      <c r="M24" s="14"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="13"/>
+      <c r="J24" s="13"/>
+      <c r="K24" s="13"/>
+      <c r="L24" s="13"/>
+      <c r="M24" s="13"/>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.5">
-      <c r="B25" s="13" t="s">
+      <c r="B25" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="C25" s="13" t="s">
+      <c r="C25" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="14"/>
-      <c r="J25" s="14"/>
-      <c r="K25" s="14"/>
-      <c r="L25" s="14"/>
-      <c r="M25" s="14"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="13"/>
+      <c r="K25" s="13"/>
+      <c r="L25" s="13"/>
+      <c r="M25" s="13"/>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.5">
-      <c r="B26" s="13" t="s">
+      <c r="B26" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="C26" s="13" t="s">
+      <c r="C26" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="14"/>
-      <c r="I26" s="14"/>
-      <c r="J26" s="14"/>
-      <c r="K26" s="14"/>
-      <c r="L26" s="14"/>
-      <c r="M26" s="14"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="13"/>
+      <c r="J26" s="13"/>
+      <c r="K26" s="13"/>
+      <c r="L26" s="13"/>
+      <c r="M26" s="13"/>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.5">
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="C27" s="13" t="s">
+      <c r="C27" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="14"/>
-      <c r="I27" s="14"/>
-      <c r="J27" s="14"/>
-      <c r="K27" s="14"/>
-      <c r="L27" s="14"/>
-      <c r="M27" s="14"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="13"/>
+      <c r="K27" s="13"/>
+      <c r="L27" s="13"/>
+      <c r="M27" s="13"/>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.5">
-      <c r="B28" s="13" t="s">
+      <c r="B28" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="C28" s="13" t="s">
+      <c r="C28" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="14"/>
-      <c r="G28" s="14"/>
-      <c r="H28" s="14"/>
-      <c r="I28" s="14"/>
-      <c r="J28" s="14"/>
-      <c r="K28" s="14"/>
-      <c r="L28" s="14"/>
-      <c r="M28" s="14"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="13"/>
+      <c r="I28" s="13"/>
+      <c r="J28" s="13"/>
+      <c r="K28" s="13"/>
+      <c r="L28" s="13"/>
+      <c r="M28" s="13"/>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.5">
-      <c r="B29" s="13" t="s">
+      <c r="B29" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="C29" s="13" t="s">
+      <c r="C29" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="14"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="14"/>
-      <c r="I29" s="14"/>
-      <c r="J29" s="14"/>
-      <c r="K29" s="14"/>
-      <c r="L29" s="14"/>
-      <c r="M29" s="14"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="13"/>
+      <c r="J29" s="13"/>
+      <c r="K29" s="13"/>
+      <c r="L29" s="13"/>
+      <c r="M29" s="13"/>
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.5">
-      <c r="B30" s="13" t="s">
+      <c r="B30" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="13" t="s">
+      <c r="C30" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D30" s="14"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="14"/>
-      <c r="G30" s="14"/>
-      <c r="H30" s="14"/>
-      <c r="I30" s="14"/>
-      <c r="J30" s="14"/>
-      <c r="K30" s="14"/>
-      <c r="L30" s="14"/>
-      <c r="M30" s="14"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="13"/>
+      <c r="I30" s="13"/>
+      <c r="J30" s="13"/>
+      <c r="K30" s="13"/>
+      <c r="L30" s="13"/>
+      <c r="M30" s="13"/>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.5">
-      <c r="B31" s="13" t="s">
+      <c r="B31" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="C31" s="13" t="s">
+      <c r="C31" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="D31" s="14"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="14"/>
-      <c r="G31" s="14"/>
-      <c r="H31" s="14"/>
-      <c r="I31" s="14"/>
-      <c r="J31" s="14"/>
-      <c r="K31" s="14"/>
-      <c r="L31" s="14"/>
-      <c r="M31" s="14"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="13"/>
+      <c r="I31" s="13"/>
+      <c r="J31" s="13"/>
+      <c r="K31" s="13"/>
+      <c r="L31" s="13"/>
+      <c r="M31" s="13"/>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.5">
-      <c r="B32" s="13" t="s">
+      <c r="B32" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="C32" s="13" t="s">
+      <c r="C32" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="14"/>
-      <c r="G32" s="14"/>
-      <c r="H32" s="14"/>
-      <c r="I32" s="14"/>
-      <c r="J32" s="14"/>
-      <c r="K32" s="14"/>
-      <c r="L32" s="14"/>
-      <c r="M32" s="14"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
+      <c r="H32" s="13"/>
+      <c r="I32" s="13"/>
+      <c r="J32" s="13"/>
+      <c r="K32" s="13"/>
+      <c r="L32" s="13"/>
+      <c r="M32" s="13"/>
     </row>
     <row r="33" spans="2:13" x14ac:dyDescent="0.5">
-      <c r="B33" s="13" t="s">
+      <c r="B33" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="C33" s="13" t="s">
+      <c r="C33" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="D33" s="14"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="14"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="14"/>
-      <c r="I33" s="14"/>
-      <c r="J33" s="14"/>
-      <c r="K33" s="14"/>
-      <c r="L33" s="14"/>
-      <c r="M33" s="14"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="13"/>
+      <c r="I33" s="13"/>
+      <c r="J33" s="13"/>
+      <c r="K33" s="13"/>
+      <c r="L33" s="13"/>
+      <c r="M33" s="13"/>
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.5">
-      <c r="B34" s="13" t="s">
+      <c r="B34" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="C34" s="13" t="s">
+      <c r="C34" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="D34" s="14"/>
-      <c r="E34" s="14"/>
-      <c r="F34" s="14"/>
-      <c r="G34" s="14"/>
-      <c r="H34" s="14"/>
-      <c r="I34" s="14"/>
-      <c r="J34" s="14"/>
-      <c r="K34" s="14"/>
-      <c r="L34" s="14"/>
-      <c r="M34" s="14"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
+      <c r="H34" s="13"/>
+      <c r="I34" s="13"/>
+      <c r="J34" s="13"/>
+      <c r="K34" s="13"/>
+      <c r="L34" s="13"/>
+      <c r="M34" s="13"/>
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.5">
-      <c r="B35" s="13" t="s">
+      <c r="B35" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="C35" s="13" t="s">
+      <c r="C35" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="D35" s="14"/>
-      <c r="E35" s="14"/>
-      <c r="F35" s="14"/>
-      <c r="G35" s="14"/>
-      <c r="H35" s="14"/>
-      <c r="I35" s="14"/>
-      <c r="J35" s="14"/>
-      <c r="K35" s="14"/>
-      <c r="L35" s="14"/>
-      <c r="M35" s="14"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="13"/>
+      <c r="I35" s="13"/>
+      <c r="J35" s="13"/>
+      <c r="K35" s="13"/>
+      <c r="L35" s="13"/>
+      <c r="M35" s="13"/>
     </row>
     <row r="36" spans="2:13" x14ac:dyDescent="0.5">
-      <c r="B36" s="13" t="s">
+      <c r="B36" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="C36" s="13" t="s">
+      <c r="C36" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="D36" s="14"/>
-      <c r="E36" s="14"/>
-      <c r="F36" s="14"/>
-      <c r="G36" s="14"/>
-      <c r="H36" s="14"/>
-      <c r="I36" s="14"/>
-      <c r="J36" s="14"/>
-      <c r="K36" s="14"/>
-      <c r="L36" s="14"/>
-      <c r="M36" s="14"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
+      <c r="H36" s="13"/>
+      <c r="I36" s="13"/>
+      <c r="J36" s="13"/>
+      <c r="K36" s="13"/>
+      <c r="L36" s="13"/>
+      <c r="M36" s="13"/>
     </row>
     <row r="37" spans="2:13" x14ac:dyDescent="0.5">
-      <c r="B37" s="13" t="s">
+      <c r="B37" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="C37" s="13" t="s">
+      <c r="C37" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="D37" s="14"/>
-      <c r="E37" s="14"/>
-      <c r="F37" s="14"/>
-      <c r="G37" s="14"/>
-      <c r="H37" s="14"/>
-      <c r="I37" s="14"/>
-      <c r="J37" s="14"/>
-      <c r="K37" s="14"/>
-      <c r="L37" s="14"/>
-      <c r="M37" s="14"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="13"/>
+      <c r="I37" s="13"/>
+      <c r="J37" s="13"/>
+      <c r="K37" s="13"/>
+      <c r="L37" s="13"/>
+      <c r="M37" s="13"/>
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.5">
-      <c r="B38" s="13" t="s">
+      <c r="B38" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="C38" s="13" t="s">
+      <c r="C38" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="D38" s="14"/>
-      <c r="E38" s="14"/>
-      <c r="F38" s="14"/>
-      <c r="G38" s="14"/>
-      <c r="H38" s="14"/>
-      <c r="I38" s="14"/>
-      <c r="J38" s="14"/>
-      <c r="K38" s="14"/>
-      <c r="L38" s="14"/>
-      <c r="M38" s="14"/>
+      <c r="D38" s="13"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="13"/>
+      <c r="G38" s="13"/>
+      <c r="H38" s="13"/>
+      <c r="I38" s="13"/>
+      <c r="J38" s="13"/>
+      <c r="K38" s="13"/>
+      <c r="L38" s="13"/>
+      <c r="M38" s="13"/>
     </row>
     <row r="39" spans="2:13" x14ac:dyDescent="0.5">
-      <c r="B39" s="13" t="s">
+      <c r="B39" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="C39" s="13" t="s">
+      <c r="C39" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="D39" s="14"/>
-      <c r="E39" s="14"/>
-      <c r="F39" s="14"/>
-      <c r="G39" s="14"/>
-      <c r="H39" s="14"/>
-      <c r="I39" s="14"/>
-      <c r="J39" s="14"/>
-      <c r="K39" s="14"/>
-      <c r="L39" s="14"/>
-      <c r="M39" s="14"/>
+      <c r="D39" s="13"/>
+      <c r="E39" s="13"/>
+      <c r="F39" s="13"/>
+      <c r="G39" s="13"/>
+      <c r="H39" s="13"/>
+      <c r="I39" s="13"/>
+      <c r="J39" s="13"/>
+      <c r="K39" s="13"/>
+      <c r="L39" s="13"/>
+      <c r="M39" s="13"/>
     </row>
     <row r="40" spans="2:13" x14ac:dyDescent="0.5">
-      <c r="B40" s="13" t="s">
+      <c r="B40" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="C40" s="13" t="s">
+      <c r="C40" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="D40" s="14"/>
-      <c r="E40" s="14"/>
-      <c r="F40" s="14"/>
-      <c r="G40" s="14"/>
-      <c r="H40" s="14"/>
-      <c r="I40" s="14"/>
-      <c r="J40" s="14"/>
-      <c r="K40" s="14"/>
-      <c r="L40" s="14"/>
-      <c r="M40" s="14"/>
+      <c r="D40" s="13"/>
+      <c r="E40" s="13"/>
+      <c r="F40" s="13"/>
+      <c r="G40" s="13"/>
+      <c r="H40" s="13"/>
+      <c r="I40" s="13"/>
+      <c r="J40" s="13"/>
+      <c r="K40" s="13"/>
+      <c r="L40" s="13"/>
+      <c r="M40" s="13"/>
     </row>
     <row r="41" spans="2:13" x14ac:dyDescent="0.5">
-      <c r="B41" s="13" t="s">
+      <c r="B41" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="C41" s="13" t="s">
+      <c r="C41" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="D41" s="14"/>
-      <c r="E41" s="14"/>
-      <c r="F41" s="14"/>
-      <c r="G41" s="14"/>
-      <c r="H41" s="14"/>
-      <c r="I41" s="14"/>
-      <c r="J41" s="14"/>
-      <c r="K41" s="14"/>
-      <c r="L41" s="14"/>
-      <c r="M41" s="14"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="13"/>
+      <c r="F41" s="13"/>
+      <c r="G41" s="13"/>
+      <c r="H41" s="13"/>
+      <c r="I41" s="13"/>
+      <c r="J41" s="13"/>
+      <c r="K41" s="13"/>
+      <c r="L41" s="13"/>
+      <c r="M41" s="13"/>
     </row>
     <row r="42" spans="2:13" x14ac:dyDescent="0.5">
-      <c r="B42" s="13" t="s">
+      <c r="B42" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="C42" s="13" t="s">
+      <c r="C42" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="D42" s="14"/>
-      <c r="E42" s="14"/>
-      <c r="F42" s="14"/>
-      <c r="G42" s="14"/>
-      <c r="H42" s="14"/>
-      <c r="I42" s="14"/>
-      <c r="J42" s="14"/>
-      <c r="K42" s="14"/>
-      <c r="L42" s="14"/>
-      <c r="M42" s="14"/>
+      <c r="D42" s="13"/>
+      <c r="E42" s="13"/>
+      <c r="F42" s="13"/>
+      <c r="G42" s="13"/>
+      <c r="H42" s="13"/>
+      <c r="I42" s="13"/>
+      <c r="J42" s="13"/>
+      <c r="K42" s="13"/>
+      <c r="L42" s="13"/>
+      <c r="M42" s="13"/>
     </row>
     <row r="43" spans="2:13" x14ac:dyDescent="0.5">
-      <c r="B43" s="13" t="s">
+      <c r="B43" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="C43" s="13" t="s">
+      <c r="C43" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="D43" s="14"/>
-      <c r="E43" s="14"/>
-      <c r="F43" s="14"/>
-      <c r="G43" s="14"/>
-      <c r="H43" s="14"/>
-      <c r="I43" s="14"/>
-      <c r="J43" s="14"/>
-      <c r="K43" s="14"/>
-      <c r="L43" s="14"/>
-      <c r="M43" s="14"/>
+      <c r="D43" s="13"/>
+      <c r="E43" s="13"/>
+      <c r="F43" s="13"/>
+      <c r="G43" s="13"/>
+      <c r="H43" s="13"/>
+      <c r="I43" s="13"/>
+      <c r="J43" s="13"/>
+      <c r="K43" s="13"/>
+      <c r="L43" s="13"/>
+      <c r="M43" s="13"/>
     </row>
     <row r="44" spans="2:13" x14ac:dyDescent="0.5">
-      <c r="B44" s="13" t="s">
+      <c r="B44" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="C44" s="13" t="s">
+      <c r="C44" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="D44" s="14"/>
-      <c r="E44" s="14"/>
-      <c r="F44" s="14"/>
-      <c r="G44" s="14"/>
-      <c r="H44" s="14"/>
-      <c r="I44" s="14"/>
-      <c r="J44" s="14"/>
-      <c r="K44" s="14"/>
-      <c r="L44" s="14"/>
-      <c r="M44" s="14"/>
+      <c r="D44" s="13"/>
+      <c r="E44" s="13"/>
+      <c r="F44" s="13"/>
+      <c r="G44" s="13"/>
+      <c r="H44" s="13"/>
+      <c r="I44" s="13"/>
+      <c r="J44" s="13"/>
+      <c r="K44" s="13"/>
+      <c r="L44" s="13"/>
+      <c r="M44" s="13"/>
     </row>
     <row r="45" spans="2:13" x14ac:dyDescent="0.5">
-      <c r="B45" s="13" t="s">
+      <c r="B45" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="C45" s="13" t="s">
+      <c r="C45" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="D45" s="14"/>
-      <c r="E45" s="14"/>
-      <c r="F45" s="14"/>
-      <c r="G45" s="14"/>
-      <c r="H45" s="14"/>
-      <c r="I45" s="14"/>
-      <c r="J45" s="14"/>
-      <c r="K45" s="14"/>
-      <c r="L45" s="14"/>
-      <c r="M45" s="14"/>
+      <c r="D45" s="13"/>
+      <c r="E45" s="13"/>
+      <c r="F45" s="13"/>
+      <c r="G45" s="13"/>
+      <c r="H45" s="13"/>
+      <c r="I45" s="13"/>
+      <c r="J45" s="13"/>
+      <c r="K45" s="13"/>
+      <c r="L45" s="13"/>
+      <c r="M45" s="13"/>
     </row>
     <row r="46" spans="2:13" x14ac:dyDescent="0.5">
-      <c r="B46" s="13" t="s">
+      <c r="B46" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="C46" s="13" t="s">
+      <c r="C46" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="D46" s="14"/>
-      <c r="E46" s="14"/>
-      <c r="F46" s="14"/>
-      <c r="G46" s="14"/>
-      <c r="H46" s="14"/>
-      <c r="I46" s="14"/>
-      <c r="J46" s="14"/>
-      <c r="K46" s="14"/>
-      <c r="L46" s="14"/>
-      <c r="M46" s="14"/>
+      <c r="D46" s="13"/>
+      <c r="E46" s="13"/>
+      <c r="F46" s="13"/>
+      <c r="G46" s="13"/>
+      <c r="H46" s="13"/>
+      <c r="I46" s="13"/>
+      <c r="J46" s="13"/>
+      <c r="K46" s="13"/>
+      <c r="L46" s="13"/>
+      <c r="M46" s="13"/>
     </row>
     <row r="47" spans="2:13" x14ac:dyDescent="0.5">
-      <c r="B47" s="13" t="s">
+      <c r="B47" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="C47" s="13" t="s">
+      <c r="C47" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="D47" s="14"/>
-      <c r="E47" s="14"/>
-      <c r="F47" s="14"/>
-      <c r="G47" s="14"/>
-      <c r="H47" s="14"/>
-      <c r="I47" s="14"/>
-      <c r="J47" s="14"/>
-      <c r="K47" s="14"/>
-      <c r="L47" s="14"/>
-      <c r="M47" s="14"/>
+      <c r="D47" s="13"/>
+      <c r="E47" s="13"/>
+      <c r="F47" s="13"/>
+      <c r="G47" s="13"/>
+      <c r="H47" s="13"/>
+      <c r="I47" s="13"/>
+      <c r="J47" s="13"/>
+      <c r="K47" s="13"/>
+      <c r="L47" s="13"/>
+      <c r="M47" s="13"/>
     </row>
     <row r="48" spans="2:13" x14ac:dyDescent="0.5">
-      <c r="B48" s="13" t="s">
+      <c r="B48" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="C48" s="13" t="s">
+      <c r="C48" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="D48" s="14"/>
-      <c r="E48" s="14"/>
-      <c r="F48" s="14"/>
-      <c r="G48" s="14"/>
-      <c r="H48" s="14"/>
-      <c r="I48" s="14"/>
-      <c r="J48" s="14"/>
-      <c r="K48" s="14"/>
-      <c r="L48" s="14"/>
-      <c r="M48" s="14"/>
+      <c r="D48" s="13"/>
+      <c r="E48" s="13"/>
+      <c r="F48" s="13"/>
+      <c r="G48" s="13"/>
+      <c r="H48" s="13"/>
+      <c r="I48" s="13"/>
+      <c r="J48" s="13"/>
+      <c r="K48" s="13"/>
+      <c r="L48" s="13"/>
+      <c r="M48" s="13"/>
     </row>
     <row r="49" spans="2:13" x14ac:dyDescent="0.5">
-      <c r="B49" s="13" t="s">
+      <c r="B49" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C49" s="13" t="s">
+      <c r="C49" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
-      <c r="H49" s="14"/>
-      <c r="I49" s="14"/>
-      <c r="J49" s="14"/>
-      <c r="K49" s="14"/>
-      <c r="L49" s="14"/>
-      <c r="M49" s="14"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="13"/>
+      <c r="G49" s="13"/>
+      <c r="H49" s="13"/>
+      <c r="I49" s="13"/>
+      <c r="J49" s="13"/>
+      <c r="K49" s="13"/>
+      <c r="L49" s="13"/>
+      <c r="M49" s="13"/>
     </row>
     <row r="50" spans="2:13" x14ac:dyDescent="0.5">
-      <c r="B50" s="13" t="s">
+      <c r="B50" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="C50" s="13" t="s">
+      <c r="C50" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="14"/>
-      <c r="G50" s="14"/>
-      <c r="H50" s="14"/>
-      <c r="I50" s="14"/>
-      <c r="J50" s="14"/>
-      <c r="K50" s="14"/>
-      <c r="L50" s="14"/>
-      <c r="M50" s="14"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="13"/>
+      <c r="G50" s="13"/>
+      <c r="H50" s="13"/>
+      <c r="I50" s="13"/>
+      <c r="J50" s="13"/>
+      <c r="K50" s="13"/>
+      <c r="L50" s="13"/>
+      <c r="M50" s="13"/>
     </row>
     <row r="51" spans="2:13" x14ac:dyDescent="0.5">
-      <c r="B51" s="13" t="s">
+      <c r="B51" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="C51" s="13" t="s">
+      <c r="C51" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="D51" s="14"/>
-      <c r="E51" s="14"/>
-      <c r="F51" s="14"/>
-      <c r="G51" s="14"/>
-      <c r="H51" s="14"/>
-      <c r="I51" s="14"/>
-      <c r="J51" s="14"/>
-      <c r="K51" s="14"/>
-      <c r="L51" s="14"/>
-      <c r="M51" s="14"/>
+      <c r="D51" s="13"/>
+      <c r="E51" s="13"/>
+      <c r="F51" s="13"/>
+      <c r="G51" s="13"/>
+      <c r="H51" s="13"/>
+      <c r="I51" s="13"/>
+      <c r="J51" s="13"/>
+      <c r="K51" s="13"/>
+      <c r="L51" s="13"/>
+      <c r="M51" s="13"/>
     </row>
     <row r="52" spans="2:13" x14ac:dyDescent="0.5">
-      <c r="B52" s="13" t="s">
+      <c r="B52" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="C52" s="13" t="s">
+      <c r="C52" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="D52" s="14"/>
-      <c r="E52" s="14"/>
-      <c r="F52" s="14"/>
-      <c r="G52" s="14"/>
-      <c r="H52" s="14"/>
-      <c r="I52" s="14"/>
-      <c r="J52" s="14"/>
-      <c r="K52" s="14"/>
-      <c r="L52" s="14"/>
-      <c r="M52" s="14"/>
+      <c r="D52" s="13"/>
+      <c r="E52" s="13"/>
+      <c r="F52" s="13"/>
+      <c r="G52" s="13"/>
+      <c r="H52" s="13"/>
+      <c r="I52" s="13"/>
+      <c r="J52" s="13"/>
+      <c r="K52" s="13"/>
+      <c r="L52" s="13"/>
+      <c r="M52" s="13"/>
     </row>
     <row r="53" spans="2:13" x14ac:dyDescent="0.5">
-      <c r="B53" s="13" t="s">
+      <c r="B53" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="C53" s="13" t="s">
+      <c r="C53" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="D53" s="14"/>
-      <c r="E53" s="14"/>
-      <c r="F53" s="14"/>
-      <c r="G53" s="14"/>
-      <c r="H53" s="14"/>
-      <c r="I53" s="14"/>
-      <c r="J53" s="14"/>
-      <c r="K53" s="14"/>
-      <c r="L53" s="14"/>
-      <c r="M53" s="14"/>
+      <c r="D53" s="13"/>
+      <c r="E53" s="13"/>
+      <c r="F53" s="13"/>
+      <c r="G53" s="13"/>
+      <c r="H53" s="13"/>
+      <c r="I53" s="13"/>
+      <c r="J53" s="13"/>
+      <c r="K53" s="13"/>
+      <c r="L53" s="13"/>
+      <c r="M53" s="13"/>
     </row>
     <row r="54" spans="2:13" x14ac:dyDescent="0.5">
-      <c r="B54" s="13" t="s">
+      <c r="B54" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="C54" s="13" t="s">
+      <c r="C54" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="D54" s="14"/>
-      <c r="E54" s="14"/>
-      <c r="F54" s="14"/>
-      <c r="G54" s="14"/>
-      <c r="H54" s="14"/>
-      <c r="I54" s="14"/>
-      <c r="J54" s="14"/>
-      <c r="K54" s="14"/>
-      <c r="L54" s="14"/>
-      <c r="M54" s="14"/>
+      <c r="D54" s="13"/>
+      <c r="E54" s="13"/>
+      <c r="F54" s="13"/>
+      <c r="G54" s="13"/>
+      <c r="H54" s="13"/>
+      <c r="I54" s="13"/>
+      <c r="J54" s="13"/>
+      <c r="K54" s="13"/>
+      <c r="L54" s="13"/>
+      <c r="M54" s="13"/>
     </row>
     <row r="55" spans="2:13" x14ac:dyDescent="0.5">
-      <c r="B55" s="13" t="s">
+      <c r="B55" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="C55" s="13" t="s">
+      <c r="C55" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="D55" s="14"/>
-      <c r="E55" s="14"/>
-      <c r="F55" s="14"/>
-      <c r="G55" s="14"/>
-      <c r="H55" s="14"/>
-      <c r="I55" s="14"/>
-      <c r="J55" s="14"/>
-      <c r="K55" s="14"/>
-      <c r="L55" s="14"/>
-      <c r="M55" s="14"/>
+      <c r="D55" s="13"/>
+      <c r="E55" s="13"/>
+      <c r="F55" s="13"/>
+      <c r="G55" s="13"/>
+      <c r="H55" s="13"/>
+      <c r="I55" s="13"/>
+      <c r="J55" s="13"/>
+      <c r="K55" s="13"/>
+      <c r="L55" s="13"/>
+      <c r="M55" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>